<commit_message>
replace feature year of birth by age , Also invert seasons for countries from the southern hemisphere
</commit_message>
<xml_diff>
--- a/results/07_plots/worst_symptom_by_season_chart.xlsx
+++ b/results/07_plots/worst_symptom_by_season_chart.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\tinnitus-country\results\07_plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7156C52-4090-4052-807E-EB88863C31E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D11B9E-1A66-4E54-969F-FE97B22E6CEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{71AE193A-8BA3-420D-AE96-943218462561}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$11:$B$27</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -201,7 +204,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16144137473141212"/>
+          <c:y val="1.4218647277596936E-2"/>
+          <c:w val="0.4516712591830121"/>
+          <c:h val="0.938672435415012"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -268,16 +281,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>6.3E-2</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.5000000000000002E-2</c:v>
+                  <c:v>6.8000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.5000000000000002E-2</c:v>
+                  <c:v>5.8999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3999999999999997E-2</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -352,16 +365,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8.6999999999999994E-2</c:v>
+                  <c:v>8.5999999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.9000000000000001E-2</c:v>
+                  <c:v>8.5000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.3000000000000004E-2</c:v>
+                  <c:v>7.4999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.8E-2</c:v>
+                  <c:v>8.2000000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -462,16 +475,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.129</c:v>
+                  <c:v>0.126</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.115</c:v>
+                  <c:v>0.126</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.124</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.105</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -546,16 +559,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.113</c:v>
+                  <c:v>0.109</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14599999999999999</c:v>
+                  <c:v>0.11600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.112</c:v>
+                  <c:v>0.14799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.127</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -630,16 +643,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.113</c:v>
+                  <c:v>0.115</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.106</c:v>
+                  <c:v>0.11600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.11799999999999999</c:v>
+                  <c:v>0.112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14499999999999999</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -714,16 +727,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.9000000000000005E-2</c:v>
+                  <c:v>0.127</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9000000000000005E-2</c:v>
+                  <c:v>9.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.123</c:v>
+                  <c:v>0.10299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11799999999999999</c:v>
+                  <c:v>0.115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -802,16 +815,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.09</c:v>
+                  <c:v>8.1000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6000000000000002E-2</c:v>
+                  <c:v>9.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.3000000000000004E-2</c:v>
+                  <c:v>9.9000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.114</c:v>
+                  <c:v>0.111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -890,13 +903,13 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.20300000000000001</c:v>
+                  <c:v>0.17899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.20200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.16800000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.17799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.16</c:v>
@@ -978,16 +991,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.10299999999999999</c:v>
+                  <c:v>0.11600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.126</c:v>
+                  <c:v>0.10100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.115</c:v>
+                  <c:v>0.127</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.109</c:v>
+                  <c:v>0.108</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1009,7 +1022,7 @@
         </c:dLbls>
         <c:dropLines>
           <c:spPr>
-            <a:ln w="9525">
+            <a:ln w="3175">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="50000"/>
@@ -1059,8 +1072,8 @@
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
@@ -1108,8 +1121,8 @@
                     <a:solidFill>
                       <a:schemeClr val="tx1"/>
                     </a:solidFill>
-                    <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
+                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
@@ -1137,8 +1150,8 @@
                   <a:solidFill>
                     <a:schemeClr val="tx1"/>
                   </a:solidFill>
-                  <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
@@ -1146,7 +1159,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1166,8 +1179,8 @@
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
-                <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
@@ -1201,12 +1214,12 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
-              <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
+              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+              <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
@@ -1249,7 +1262,8 @@
           <a:solidFill>
             <a:schemeClr val="tx1"/>
           </a:solidFill>
-          <a:latin typeface="Bodoni MT" panose="02070603080606020203" pitchFamily="18" charset="0"/>
+          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
         </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
@@ -1807,16 +1821,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>582175</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>164625</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>521663</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>57797</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>448236</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>329495</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>181536</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>222666</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2143,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5018F508-4C00-454F-AD85-125A5274D41F}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="60" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2174,16 +2188,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>6.3E-2</v>
+        <v>0.06</v>
       </c>
       <c r="C2" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="D2" s="2">
-        <v>6.5000000000000002E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="E2" s="2">
-        <v>4.3999999999999997E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2191,16 +2205,16 @@
         <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>8.6999999999999994E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="C3" s="2">
-        <v>7.9000000000000001E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="D3" s="2">
-        <v>8.3000000000000004E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="E3" s="2">
-        <v>7.8E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2208,16 +2222,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="2">
-        <v>0.129</v>
+        <v>0.126</v>
       </c>
       <c r="C4" s="2">
-        <v>0.115</v>
+        <v>0.126</v>
       </c>
       <c r="D4" s="2">
-        <v>0.124</v>
+        <v>0.11</v>
       </c>
       <c r="E4" s="2">
-        <v>0.105</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2225,16 +2239,16 @@
         <v>9</v>
       </c>
       <c r="B5" s="2">
-        <v>0.113</v>
+        <v>0.109</v>
       </c>
       <c r="C5" s="2">
-        <v>0.14599999999999999</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="D5" s="2">
-        <v>0.112</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="E5" s="2">
-        <v>0.127</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2242,16 +2256,16 @@
         <v>10</v>
       </c>
       <c r="B6" s="2">
-        <v>0.113</v>
+        <v>0.115</v>
       </c>
       <c r="C6" s="2">
-        <v>0.106</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="D6" s="2">
-        <v>0.11799999999999999</v>
+        <v>0.112</v>
       </c>
       <c r="E6" s="2">
-        <v>0.14499999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2259,16 +2273,16 @@
         <v>11</v>
       </c>
       <c r="B7" s="2">
-        <v>9.9000000000000005E-2</v>
+        <v>0.127</v>
       </c>
       <c r="C7" s="2">
-        <v>9.9000000000000005E-2</v>
+        <v>9.4E-2</v>
       </c>
       <c r="D7" s="2">
-        <v>0.123</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="E7" s="2">
-        <v>0.11799999999999999</v>
+        <v>0.115</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2276,16 +2290,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>0.09</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="C8" s="2">
-        <v>9.6000000000000002E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="D8" s="2">
-        <v>8.3000000000000004E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="E8" s="2">
-        <v>0.114</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -2293,13 +2307,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="2">
-        <v>0.20300000000000001</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="C9" s="2">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="D9" s="2">
         <v>0.16800000000000001</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.17799999999999999</v>
       </c>
       <c r="E9" s="2">
         <v>0.16</v>
@@ -2310,16 +2324,16 @@
         <v>13</v>
       </c>
       <c r="B10" s="2">
-        <v>0.10299999999999999</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="C10" s="2">
-        <v>0.126</v>
+        <v>0.10100000000000001</v>
       </c>
       <c r="D10" s="2">
-        <v>0.115</v>
+        <v>0.127</v>
       </c>
       <c r="E10" s="2">
-        <v>0.109</v>
+        <v>0.108</v>
       </c>
     </row>
   </sheetData>
@@ -2336,6 +2350,7 @@
     <cfRule type="top10" dxfId="0" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="98" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
report results about assesment-level approach for tinnitus classification on static features
accuracy on test set 84%
</commit_message>
<xml_diff>
--- a/results/07_plots/worst_symptom_by_season_chart.xlsx
+++ b/results/07_plots/worst_symptom_by_season_chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joa24jm\Documents\tinnitus-country\results\07_plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F061931-3010-4B0B-A003-9A572B55195E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC443D3C-A339-4F82-8A08-ECE6D629BE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15220" yWindow="-14510" windowWidth="51420" windowHeight="14020" xr2:uid="{71AE193A-8BA3-420D-AE96-943218462561}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{71AE193A-8BA3-420D-AE96-943218462561}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4179,7 +4179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5018F508-4C00-454F-AD85-125A5274D41F}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="85" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>